<commit_message>
sentence parser bug fixes 2022-11-20
</commit_message>
<xml_diff>
--- a/data/NOTAM_table.xlsx
+++ b/data/NOTAM_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workstation\data\NOTAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429ABC3A-3D7C-46C5-BBD8-E717EC84B1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD98FA4-9C9B-4269-8303-429BBD43ED32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,14 +21,14 @@
     <sheet name="limit_list" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">words_list!$A$1:$A$141</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">words_list!$A$1:$C$144</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="238">
   <si>
     <t>before</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>APCH ONLY</t>
-  </si>
-  <si>
-    <t>APV ONLY</t>
   </si>
   <si>
     <t>ARE ADVISED TO</t>
@@ -3104,14 +3101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(?=(-.*(ARR|DEP)(/*)(ARR|DEP)*)|((TKOF|LDG)(/*)(TKOF|LDG)*))(?P&lt;limit&gt;.*ONLY.*)</t>
-    <phoneticPr fontId="29" type="noConversion"/>
-  </si>
-  <si>
-    <t>(WITH|MAX).*WINGSPAN</t>
-    <phoneticPr fontId="29" type="noConversion"/>
-  </si>
-  <si>
     <t>NOT USEFUL</t>
   </si>
   <si>
@@ -3473,13 +3462,41 @@
   <si>
     <t>BY CALIBRATION UNIT</t>
     <phoneticPr fontId="29" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVBL PN</t>
+  </si>
+  <si>
+    <t>LOCALLY DECREASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARR/DEP WITH </t>
+    <phoneticPr fontId="29" type="noConversion"/>
+  </si>
+  <si>
+    <t>(WITH|MAX).*(WINGSPAN|WING SPAN)</t>
+    <phoneticPr fontId="29" type="noConversion"/>
+  </si>
+  <si>
+    <t>ONLY AVBL</t>
+    <phoneticPr fontId="29" type="noConversion"/>
+  </si>
+  <si>
+    <t>(?=(-.*(ARR|DEP)(/*)(ARR|DEP)*)|((TKOF|LDG)(/*)(TKOF|LDG)*))(?P&lt;limit&gt;.*ONLY.*)</t>
+  </si>
+  <si>
+    <t>(?=(-.*(ARR|DEP)(/*)(ARR|DEP)*)|((TKOF|LDG)(/*)(TKOF|LDG)*)|((ARR|DEP)(/*)(ARR|DEP)*))(?P&lt;limit&gt;.*ONLY.*)</t>
+    <phoneticPr fontId="29" type="noConversion"/>
+  </si>
+  <si>
+    <t>APV ONLY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3690,31 +3707,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -3722,23 +3714,15 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3771,6 +3755,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF8CDDFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3819,7 +3815,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3865,49 +3861,64 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4252,8 +4263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4266,14 +4277,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>205</v>
+      <c r="C1" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4282,13 +4293,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1"/>
@@ -4298,13 +4309,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="1"/>
@@ -4314,1199 +4325,1213 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="21"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="14"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="21"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="21"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="21"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="21"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" s="17"/>
+      <c r="B13" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" s="21"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="21"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="21"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="C16" s="21"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="21"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="C18" s="21"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="C20" s="21"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="17"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="B34" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="B35" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C38" s="21"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="21"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="21"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="21"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="C36" s="17"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="17"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="17"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="17"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="17"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="17"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="21"/>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="21"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="21"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="17"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="21"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="17"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="21"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="17"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="B47" s="15"/>
+      <c r="C47" s="21"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="17"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="B48" s="15"/>
+      <c r="C48" s="21"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="17"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="21"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="21"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="17"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="17"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="17"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="17"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="21"/>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="21"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" s="15"/>
+      <c r="C53" s="21"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="15"/>
+      <c r="C54" s="21"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="21"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="17"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="B56" s="15"/>
+      <c r="C56" s="21"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="17"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="B57" s="15"/>
+      <c r="C57" s="21"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="17"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+      <c r="B58" s="15"/>
+      <c r="C58" s="21"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="21"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="17"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+      <c r="B60" s="15"/>
+      <c r="C60" s="21"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="17"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="17"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="17"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="25"/>
-      <c r="C59" s="17"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="17"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="21"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="17"/>
+        <v>215</v>
+      </c>
+      <c r="B62" s="15"/>
+      <c r="C62" s="21"/>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="21"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="21"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="21"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="15"/>
+      <c r="C66" s="21"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="17"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="B67" s="15"/>
+      <c r="C67" s="21"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="17"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="B68" s="15"/>
+      <c r="C68" s="21"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="17"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="B69" s="15"/>
+      <c r="C69" s="21"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B66" s="25"/>
-      <c r="C66" s="17"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="B70" s="15"/>
+      <c r="C70" s="21"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="25"/>
-      <c r="C67" s="17"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="B71" s="15"/>
+      <c r="C71" s="21"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B68" s="25"/>
-      <c r="C68" s="17"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="B72" s="15"/>
+      <c r="C72" s="21"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B69" s="25"/>
-      <c r="C69" s="17"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+      <c r="B73" s="15"/>
+      <c r="C73" s="21"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="25"/>
-      <c r="C70" s="17"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="B74" s="15"/>
+      <c r="C74" s="21"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="25"/>
-      <c r="C71" s="17"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+      <c r="B75" s="15"/>
+      <c r="C75" s="21"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B72" s="25"/>
-      <c r="C72" s="17"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+      <c r="B76" s="15"/>
+      <c r="C76" s="21"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B73" s="25"/>
-      <c r="C73" s="17"/>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="B77" s="15"/>
+      <c r="C77" s="21"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B74" s="25"/>
-      <c r="C74" s="17"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="B78" s="15"/>
+      <c r="C78" s="21"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="25"/>
-      <c r="C75" s="17"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B76" s="25"/>
-      <c r="C76" s="17"/>
-      <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="17"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="17"/>
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="17"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="21"/>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="25"/>
-      <c r="C80" s="17"/>
+      <c r="A80" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B80" s="15"/>
+      <c r="C80" s="21"/>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B81" s="25"/>
-      <c r="C81" s="17"/>
+        <v>234</v>
+      </c>
+      <c r="B81" s="15"/>
+      <c r="C81" s="21"/>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" s="25"/>
-      <c r="C82" s="17"/>
+      <c r="A82" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="15"/>
+      <c r="C82" s="21"/>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B83" s="25"/>
-      <c r="C83" s="17"/>
+      <c r="A83" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="15"/>
+      <c r="C83" s="21"/>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B84" s="25"/>
-      <c r="C84" s="17"/>
+      <c r="A84" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="15"/>
+      <c r="C84" s="21"/>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B85" s="25"/>
-      <c r="C85" s="17"/>
+        <v>132</v>
+      </c>
+      <c r="B85" s="15"/>
+      <c r="C85" s="21"/>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B86" s="25"/>
-      <c r="C86" s="17"/>
+      <c r="A86" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="15"/>
+      <c r="C86" s="21"/>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B87" s="25"/>
-      <c r="C87" s="17"/>
+      <c r="A87" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="15"/>
+      <c r="C87" s="21"/>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="25"/>
-      <c r="C88" s="17"/>
+      <c r="A88" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" s="15"/>
+      <c r="C88" s="21"/>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B89" s="25"/>
-      <c r="C89" s="17"/>
+        <v>136</v>
+      </c>
+      <c r="B89" s="15"/>
+      <c r="C89" s="21"/>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B90" s="25"/>
-      <c r="C90" s="17"/>
+      <c r="A90" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="C90" s="21"/>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="17"/>
+      <c r="A91" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="15"/>
+      <c r="C91" s="21"/>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B92" s="25"/>
-      <c r="C92" s="17"/>
+      <c r="A92" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="15"/>
+      <c r="C92" s="21"/>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B93" s="25"/>
-      <c r="C93" s="17"/>
+      <c r="A93" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" s="15"/>
+      <c r="C93" s="21"/>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B94" s="25"/>
-      <c r="C94" s="17"/>
+      <c r="A94" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="15"/>
+      <c r="C94" s="21"/>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95" s="15"/>
+      <c r="C95" s="21"/>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B96" s="15"/>
+      <c r="C96" s="21"/>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="B97" s="15"/>
+      <c r="C97" s="21"/>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B98" s="15"/>
+      <c r="C98" s="21"/>
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="15"/>
+      <c r="C99" s="21"/>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="15"/>
+      <c r="C100" s="21"/>
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="15"/>
+      <c r="C101" s="21"/>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B95" s="25"/>
-      <c r="C95" s="17"/>
-      <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B96" s="25"/>
-      <c r="C96" s="17"/>
-      <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B97" s="25"/>
-      <c r="C97" s="17"/>
-      <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="B98" s="25"/>
-      <c r="C98" s="17"/>
-      <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B99" s="25"/>
-      <c r="C99" s="17"/>
-      <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B100" s="25"/>
-      <c r="C100" s="17"/>
-      <c r="E100" s="1"/>
-    </row>
-    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="B101" s="25"/>
-      <c r="C101" s="17"/>
-      <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B102" s="25"/>
-      <c r="C102" s="17"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="21"/>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B103" s="15"/>
+      <c r="C103" s="21"/>
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="B104" s="15"/>
+      <c r="C104" s="21"/>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105" s="15"/>
+      <c r="C105" s="21"/>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B106" s="15"/>
+      <c r="C106" s="21"/>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B107" s="15"/>
+      <c r="C107" s="21"/>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" s="15"/>
+      <c r="C108" s="21"/>
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" s="15"/>
+      <c r="C109" s="21"/>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" s="15"/>
+      <c r="C110" s="21"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" s="15"/>
+      <c r="C111" s="21"/>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" s="15"/>
+      <c r="C112" s="21"/>
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B103" s="25"/>
-      <c r="C103" s="17"/>
-      <c r="E103" s="1"/>
-    </row>
-    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+      <c r="B113" s="15"/>
+      <c r="C113" s="21"/>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B104" s="25"/>
-      <c r="C104" s="17"/>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+      <c r="B114" s="15"/>
+      <c r="C114" s="21"/>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="B105" s="25"/>
-      <c r="C105" s="17"/>
-      <c r="E105" s="1"/>
-    </row>
-    <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="22" t="s">
+      <c r="B115" s="15"/>
+      <c r="C115" s="21"/>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B106" s="25"/>
-      <c r="C106" s="17"/>
-      <c r="E106" s="1"/>
-    </row>
-    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="19" t="s">
+      <c r="B116" s="15"/>
+      <c r="C116" s="21"/>
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="15"/>
+      <c r="C117" s="21"/>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="B107" s="25"/>
-      <c r="C107" s="17"/>
-      <c r="E107" s="1"/>
-    </row>
-    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="19" t="s">
+      <c r="B118" s="15"/>
+      <c r="C118" s="21"/>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119" s="15"/>
+      <c r="C119" s="21"/>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B108" s="25"/>
-      <c r="C108" s="17"/>
-      <c r="E108" s="1"/>
-    </row>
-    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="19" t="s">
+      <c r="B120" s="15"/>
+      <c r="C120" s="21"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="17"/>
-      <c r="E109" s="1"/>
-    </row>
-    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="19" t="s">
+      <c r="B121" s="15"/>
+      <c r="C121" s="21"/>
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="17"/>
-      <c r="E110" s="1"/>
-    </row>
-    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="19" t="s">
+      <c r="B122" s="15"/>
+      <c r="C122" s="21"/>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="17"/>
-      <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="25" t="s">
+      <c r="B123" s="15"/>
+      <c r="C123" s="21"/>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="17"/>
-      <c r="E112" s="1"/>
-    </row>
-    <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="19" t="s">
+      <c r="B124" s="15"/>
+      <c r="C124" s="21"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="B113" s="25"/>
-      <c r="C113" s="17"/>
-      <c r="E113" s="1"/>
-    </row>
-    <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="19" t="s">
+      <c r="B125" s="15"/>
+      <c r="C125" s="21"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B114" s="25"/>
-      <c r="C114" s="17"/>
-      <c r="E114" s="1"/>
-    </row>
-    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="19" t="s">
+      <c r="B126" s="15"/>
+      <c r="C126" s="21"/>
+      <c r="E126" s="1"/>
+    </row>
+    <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B115" s="25"/>
-      <c r="C115" s="17"/>
-      <c r="E115" s="1"/>
-    </row>
-    <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="19" t="s">
+      <c r="B127" s="15"/>
+      <c r="C127" s="21"/>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B116" s="25"/>
-      <c r="C116" s="17"/>
-      <c r="E116" s="1"/>
-    </row>
-    <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117" s="19" t="s">
+      <c r="B128" s="15"/>
+      <c r="C128" s="21"/>
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B117" s="25"/>
-      <c r="C117" s="17"/>
-      <c r="E117" s="1"/>
-    </row>
-    <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="19" t="s">
+      <c r="B129" s="15"/>
+      <c r="C129" s="21"/>
+      <c r="E129" s="1"/>
+    </row>
+    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B118" s="20"/>
-      <c r="C118" s="17"/>
-      <c r="E118" s="1"/>
-    </row>
-    <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="19" t="s">
+      <c r="B130" s="15"/>
+      <c r="C130" s="21"/>
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B119" s="20"/>
-      <c r="C119" s="17"/>
-      <c r="E119" s="1"/>
-    </row>
-    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A120" s="25" t="s">
+      <c r="B131" s="15"/>
+      <c r="C131" s="21"/>
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B120" s="20"/>
-      <c r="C120" s="17"/>
-      <c r="E120" s="1"/>
-    </row>
-    <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="19" t="s">
+      <c r="B132" s="15"/>
+      <c r="C132" s="21"/>
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="B121" s="20"/>
-      <c r="C121" s="17"/>
-      <c r="E121" s="1"/>
-    </row>
-    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="19" t="s">
+      <c r="B133" s="15"/>
+      <c r="C133" s="21"/>
+      <c r="E133" s="1"/>
+    </row>
+    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="B122" s="20"/>
-      <c r="C122" s="17"/>
-      <c r="E122" s="1"/>
-    </row>
-    <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123" s="19" t="s">
+      <c r="B134" s="15"/>
+      <c r="C134" s="21"/>
+      <c r="E134" s="1"/>
+    </row>
+    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B123" s="20"/>
-      <c r="C123" s="17"/>
-      <c r="E123" s="1"/>
-    </row>
-    <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A124" s="25" t="s">
+      <c r="B135" s="15"/>
+      <c r="C135" s="21"/>
+      <c r="E135" s="1"/>
+    </row>
+    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B124" s="20"/>
-      <c r="C124" s="17"/>
-      <c r="E124" s="1"/>
-    </row>
-    <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" s="19" t="s">
+      <c r="B136" s="15"/>
+      <c r="C136" s="21"/>
+      <c r="E136" s="1"/>
+    </row>
+    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="B125" s="20"/>
-      <c r="C125" s="17"/>
-      <c r="E125" s="1"/>
-    </row>
-    <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="19" t="s">
+      <c r="B137" s="15"/>
+      <c r="C137" s="21"/>
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="B126" s="20"/>
-      <c r="C126" s="17"/>
-      <c r="E126" s="1"/>
-    </row>
-    <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" s="25" t="s">
+      <c r="B138" s="15"/>
+      <c r="C138" s="21"/>
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B127" s="20"/>
-      <c r="C127" s="17"/>
-      <c r="E127" s="1"/>
-    </row>
-    <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A128" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B128" s="20"/>
-      <c r="C128" s="17"/>
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A129" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="B129" s="20"/>
-      <c r="C129" s="17"/>
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A130" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="B130" s="20"/>
-      <c r="C130" s="17"/>
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A131" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="B131" s="20"/>
-      <c r="C131" s="17"/>
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B132" s="20"/>
-      <c r="C132" s="17"/>
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A133" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="B133" s="20"/>
-      <c r="C133" s="17"/>
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="B134" s="20"/>
-      <c r="C134" s="17"/>
-      <c r="E134" s="1"/>
-    </row>
-    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A135" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="B135" s="20"/>
-      <c r="C135" s="17"/>
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="B136" s="20"/>
-      <c r="C136" s="17"/>
-      <c r="E136" s="1"/>
-    </row>
-    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="B137" s="20"/>
-      <c r="C137" s="17"/>
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A138" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B138" s="20"/>
-      <c r="C138" s="17"/>
-      <c r="E138" s="1"/>
-    </row>
-    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="B139" s="20"/>
-      <c r="C139" s="17"/>
+      <c r="B139" s="15"/>
+      <c r="C139" s="21"/>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B140" s="20"/>
-      <c r="C140" s="17"/>
+        <v>184</v>
+      </c>
+      <c r="B140" s="15"/>
+      <c r="C140" s="21"/>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A141" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="B141" s="20"/>
-      <c r="C141" s="17"/>
+      <c r="A141" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B141" s="15"/>
+      <c r="C141" s="21"/>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>223</v>
-      </c>
-      <c r="B142" s="1"/>
+      <c r="A142" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B142" s="15"/>
+      <c r="C142" s="21"/>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>231</v>
-      </c>
-      <c r="B143" s="1"/>
+      <c r="A143" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B143" s="15"/>
+      <c r="C143" s="21"/>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B144" s="1"/>
+      <c r="A144" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B144" s="15"/>
+      <c r="C144" s="21"/>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="1"/>
+      <c r="B145" s="15"/>
+      <c r="C145" s="21"/>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -5722,9 +5747,10 @@
       <c r="E198" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A141" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C144" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="29" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5733,7 +5759,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5756,7 +5782,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -5767,7 +5793,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
@@ -5778,7 +5804,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>2</v>
@@ -5789,7 +5815,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>34</v>
@@ -5799,8 +5825,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>194</v>
+      <c r="A6" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>35</v>
@@ -5811,7 +5837,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>35</v>
@@ -5821,8 +5847,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>218</v>
+      <c r="A8" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>35</v>
@@ -5833,7 +5859,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>36</v>
@@ -5850,6 +5876,7 @@
   </sheetData>
   <phoneticPr fontId="29" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5880,7 +5907,7 @@
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
@@ -5891,7 +5918,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -5908,9 +5935,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5931,18 +5960,18 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -5950,10 +5979,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -5974,7 +6003,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -5998,14 +6027,19 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="29" type="noConversion"/>

</xml_diff>

<commit_message>
sentense parser update 2022-11-20 XMU CZY
</commit_message>
<xml_diff>
--- a/data/NOTAM_table.xlsx
+++ b/data/NOTAM_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workstation\data\NOTAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD98FA4-9C9B-4269-8303-429BBD43ED32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5052C7-A825-4F73-AF6E-5674D07D742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="15360" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words_list" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="237">
   <si>
     <t>before</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>PERMITTED</t>
-  </si>
-  <si>
-    <t>PLAN</t>
   </si>
   <si>
     <t>PROHIBITED</t>
@@ -3815,7 +3812,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3900,25 +3897,13 @@
     <xf numFmtId="0" fontId="31" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4261,10 +4246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4284,7 +4270,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4292,12 +4278,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>206</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>10</v>
@@ -4308,12 +4294,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>207</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>208</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>40</v>
@@ -4324,31 +4310,31 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>45</v>
       </c>
@@ -4360,7 +4346,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>46</v>
       </c>
@@ -4370,7 +4356,7 @@
       <c r="C7" s="21"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>48</v>
       </c>
@@ -4381,7 +4367,7 @@
       <c r="D8" s="14"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>50</v>
       </c>
@@ -4391,7 +4377,7 @@
       <c r="C9" s="21"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>52</v>
       </c>
@@ -4401,17 +4387,17 @@
       <c r="C10" s="21"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="21"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>56</v>
       </c>
@@ -4421,27 +4407,27 @@
       <c r="C12" s="21"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" s="21"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="21"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>60</v>
       </c>
@@ -4451,9 +4437,9 @@
       <c r="C15" s="21"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>61</v>
@@ -4461,7 +4447,7 @@
       <c r="C16" s="21"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>62</v>
       </c>
@@ -4471,9 +4457,9 @@
       <c r="C17" s="21"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>64</v>
@@ -4481,7 +4467,7 @@
       <c r="C18" s="21"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>65</v>
       </c>
@@ -4491,9 +4477,9 @@
       <c r="C19" s="21"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>67</v>
@@ -4501,7 +4487,7 @@
       <c r="C20" s="21"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>68</v>
       </c>
@@ -4511,7 +4497,7 @@
       <c r="C21" s="21"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>70</v>
       </c>
@@ -4521,7 +4507,7 @@
       <c r="C22" s="21"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>72</v>
       </c>
@@ -4531,7 +4517,7 @@
       <c r="C23" s="21"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>74</v>
       </c>
@@ -4541,7 +4527,7 @@
       <c r="C24" s="21"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>76</v>
       </c>
@@ -4551,7 +4537,7 @@
       <c r="C25" s="21"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>78</v>
       </c>
@@ -4561,47 +4547,47 @@
       <c r="C26" s="21"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="15" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="21"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="15" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="21"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="21"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C30" s="21"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>86</v>
       </c>
@@ -4611,77 +4597,77 @@
       <c r="C31" s="21"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="33" t="s">
-        <v>233</v>
+      <c r="B32" s="29" t="s">
+        <v>232</v>
       </c>
       <c r="C32" s="21"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>89</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C33" s="21"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>226</v>
+        <v>212</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>225</v>
       </c>
       <c r="C34" s="21"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>90</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C35" s="21"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C36" s="21"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="31" t="s">
-        <v>237</v>
+      <c r="B37" s="21" t="s">
+        <v>236</v>
       </c>
       <c r="C37" s="21"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C38" s="21"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>94</v>
       </c>
@@ -4689,7 +4675,7 @@
       <c r="C39" s="21"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>95</v>
       </c>
@@ -4697,7 +4683,7 @@
       <c r="C40" s="21"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>96</v>
       </c>
@@ -4705,23 +4691,23 @@
       <c r="C41" s="21"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="21"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="21"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>97</v>
       </c>
@@ -4729,7 +4715,7 @@
       <c r="C44" s="21"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>98</v>
       </c>
@@ -4737,7 +4723,7 @@
       <c r="C45" s="21"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>99</v>
       </c>
@@ -4745,7 +4731,7 @@
       <c r="C46" s="21"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>100</v>
       </c>
@@ -4753,7 +4739,7 @@
       <c r="C47" s="21"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>101</v>
       </c>
@@ -4761,7 +4747,7 @@
       <c r="C48" s="21"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>102</v>
       </c>
@@ -4769,7 +4755,7 @@
       <c r="C49" s="21"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>102</v>
       </c>
@@ -4777,7 +4763,7 @@
       <c r="C50" s="21"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>103</v>
       </c>
@@ -4785,23 +4771,23 @@
       <c r="C51" s="21"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="21"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
-        <v>231</v>
+    <row r="53" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
+        <v>230</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="21"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>104</v>
       </c>
@@ -4809,7 +4795,7 @@
       <c r="C54" s="21"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>105</v>
       </c>
@@ -4817,7 +4803,7 @@
       <c r="C55" s="21"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>106</v>
       </c>
@@ -4825,7 +4811,7 @@
       <c r="C56" s="21"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>107</v>
       </c>
@@ -4833,7 +4819,7 @@
       <c r="C57" s="21"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>108</v>
       </c>
@@ -4841,15 +4827,15 @@
       <c r="C58" s="21"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B59" s="15"/>
       <c r="C59" s="21"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>109</v>
       </c>
@@ -4857,7 +4843,7 @@
       <c r="C60" s="21"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>110</v>
       </c>
@@ -4865,15 +4851,15 @@
       <c r="C61" s="21"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="21"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>112</v>
       </c>
@@ -4881,7 +4867,7 @@
       <c r="C63" s="21"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>113</v>
       </c>
@@ -4889,7 +4875,7 @@
       <c r="C64" s="21"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>114</v>
       </c>
@@ -4897,7 +4883,7 @@
       <c r="C65" s="21"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>115</v>
       </c>
@@ -4905,7 +4891,7 @@
       <c r="C66" s="21"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>116</v>
       </c>
@@ -4913,7 +4899,7 @@
       <c r="C67" s="21"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>117</v>
       </c>
@@ -4921,7 +4907,7 @@
       <c r="C68" s="21"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>118</v>
       </c>
@@ -4929,7 +4915,7 @@
       <c r="C69" s="21"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>119</v>
       </c>
@@ -4937,7 +4923,7 @@
       <c r="C70" s="21"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>120</v>
       </c>
@@ -4945,7 +4931,7 @@
       <c r="C71" s="21"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>121</v>
       </c>
@@ -4953,7 +4939,7 @@
       <c r="C72" s="21"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>122</v>
       </c>
@@ -4961,7 +4947,7 @@
       <c r="C73" s="21"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>123</v>
       </c>
@@ -4969,7 +4955,7 @@
       <c r="C74" s="21"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>124</v>
       </c>
@@ -4977,7 +4963,7 @@
       <c r="C75" s="21"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>125</v>
       </c>
@@ -4985,7 +4971,7 @@
       <c r="C76" s="21"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>126</v>
       </c>
@@ -4993,7 +4979,7 @@
       <c r="C77" s="21"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
         <v>127</v>
       </c>
@@ -5001,7 +4987,7 @@
       <c r="C78" s="21"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
         <v>128</v>
       </c>
@@ -5009,23 +4995,23 @@
       <c r="C79" s="21"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B80" s="15"/>
       <c r="C80" s="21"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B81" s="15"/>
       <c r="C81" s="21"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
         <v>129</v>
       </c>
@@ -5033,7 +5019,7 @@
       <c r="C82" s="21"/>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>130</v>
       </c>
@@ -5041,7 +5027,7 @@
       <c r="C83" s="21"/>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>131</v>
       </c>
@@ -5049,7 +5035,7 @@
       <c r="C84" s="21"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
         <v>132</v>
       </c>
@@ -5057,7 +5043,7 @@
       <c r="C85" s="21"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
         <v>133</v>
       </c>
@@ -5065,7 +5051,7 @@
       <c r="C86" s="21"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
         <v>134</v>
       </c>
@@ -5073,7 +5059,7 @@
       <c r="C87" s="21"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
         <v>135</v>
       </c>
@@ -5081,7 +5067,7 @@
       <c r="C88" s="21"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
         <v>136</v>
       </c>
@@ -5089,7 +5075,7 @@
       <c r="C89" s="21"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
         <v>137</v>
       </c>
@@ -5098,432 +5084,430 @@
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="20" t="s">
-        <v>138</v>
-      </c>
+      <c r="A91" s="20"/>
       <c r="B91" s="15"/>
       <c r="C91" s="21"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="21"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B93" s="15"/>
       <c r="C93" s="21"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B94" s="15"/>
       <c r="C94" s="21"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B95" s="15"/>
       <c r="C95" s="21"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" s="15"/>
       <c r="C96" s="21"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
-        <v>228</v>
+    <row r="97" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="B97" s="15"/>
       <c r="C97" s="21"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B98" s="15"/>
       <c r="C98" s="21"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B99" s="15"/>
       <c r="C99" s="21"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B100" s="15"/>
       <c r="C100" s="21"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B101" s="15"/>
       <c r="C101" s="21"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="21"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B103" s="15"/>
       <c r="C103" s="21"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
-        <v>220</v>
+    <row r="104" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="28" t="s">
+        <v>219</v>
       </c>
       <c r="B104" s="15"/>
       <c r="C104" s="21"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B105" s="15"/>
       <c r="C105" s="21"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="28" t="s">
-        <v>150</v>
+    <row r="106" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="B106" s="15"/>
       <c r="C106" s="21"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B107" s="15"/>
       <c r="C107" s="21"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="29" t="s">
-        <v>151</v>
+    <row r="108" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="26" t="s">
+        <v>150</v>
       </c>
       <c r="B108" s="15"/>
       <c r="C108" s="21"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="29" t="s">
-        <v>152</v>
+    <row r="109" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="26" t="s">
+        <v>151</v>
       </c>
       <c r="B109" s="15"/>
       <c r="C109" s="21"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
-        <v>153</v>
+    <row r="110" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="B110" s="15"/>
       <c r="C110" s="21"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="29" t="s">
-        <v>154</v>
+    <row r="111" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="26" t="s">
+        <v>153</v>
       </c>
       <c r="B111" s="15"/>
       <c r="C111" s="21"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="29" t="s">
-        <v>155</v>
+    <row r="112" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="26" t="s">
+        <v>154</v>
       </c>
       <c r="B112" s="15"/>
       <c r="C112" s="21"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="29" t="s">
-        <v>156</v>
+    <row r="113" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="26" t="s">
+        <v>155</v>
       </c>
       <c r="B113" s="15"/>
       <c r="C113" s="21"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="29" t="s">
-        <v>157</v>
+    <row r="114" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="21"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="28" t="s">
-        <v>158</v>
+    <row r="115" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="B115" s="15"/>
       <c r="C115" s="21"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B116" s="15"/>
       <c r="C116" s="21"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B117" s="15"/>
       <c r="C117" s="21"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B118" s="15"/>
       <c r="C118" s="21"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A119" s="28" t="s">
+    <row r="119" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
         <v>111</v>
       </c>
       <c r="B119" s="15"/>
       <c r="C119" s="21"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B120" s="15"/>
       <c r="C120" s="21"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B121" s="15"/>
       <c r="C121" s="21"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B122" s="15"/>
       <c r="C122" s="21"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B123" s="15"/>
       <c r="C123" s="21"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B124" s="15"/>
       <c r="C124" s="21"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B125" s="15"/>
       <c r="C125" s="21"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B126" s="15"/>
       <c r="C126" s="21"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B127" s="15"/>
       <c r="C127" s="21"/>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B128" s="15"/>
       <c r="C128" s="21"/>
       <c r="E128" s="1"/>
     </row>
-    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B129" s="15"/>
       <c r="C129" s="21"/>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B130" s="15"/>
       <c r="C130" s="21"/>
       <c r="E130" s="1"/>
     </row>
-    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B131" s="15"/>
       <c r="C131" s="21"/>
       <c r="E131" s="1"/>
     </row>
-    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B132" s="15"/>
       <c r="C132" s="21"/>
       <c r="E132" s="1"/>
     </row>
-    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B133" s="15"/>
       <c r="C133" s="21"/>
       <c r="E133" s="1"/>
     </row>
-    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B134" s="15"/>
       <c r="C134" s="21"/>
       <c r="E134" s="1"/>
     </row>
-    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B135" s="15"/>
       <c r="C135" s="21"/>
       <c r="E135" s="1"/>
     </row>
-    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B136" s="15"/>
       <c r="C136" s="21"/>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B137" s="15"/>
       <c r="C137" s="21"/>
       <c r="E137" s="1"/>
     </row>
-    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B138" s="15"/>
       <c r="C138" s="21"/>
       <c r="E138" s="1"/>
     </row>
-    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B139" s="15"/>
       <c r="C139" s="21"/>
       <c r="E139" s="1"/>
     </row>
-    <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B140" s="15"/>
       <c r="C140" s="21"/>
       <c r="E140" s="1"/>
     </row>
-    <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B141" s="15"/>
       <c r="C141" s="21"/>
       <c r="E141" s="1"/>
     </row>
-    <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B142" s="15"/>
       <c r="C142" s="21"/>
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B143" s="15"/>
       <c r="C143" s="21"/>
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B144" s="15"/>
       <c r="C144" s="21"/>
@@ -5747,7 +5731,13 @@
       <c r="E198" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C144" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C144" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="PLAN"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="29" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5782,7 +5772,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -5793,7 +5783,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
@@ -5804,7 +5794,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>2</v>
@@ -5815,7 +5805,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>34</v>
@@ -5826,7 +5816,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>35</v>
@@ -5837,7 +5827,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>35</v>
@@ -5848,7 +5838,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>35</v>
@@ -5859,7 +5849,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>36</v>
@@ -5907,7 +5897,7 @@
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
@@ -5918,7 +5908,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -5960,18 +5950,18 @@
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -5979,10 +5969,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -6003,7 +5993,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -6027,10 +6017,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -6038,7 +6028,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>